<commit_message>
Spring Boot JPA Query execution
Spring Boot JPA Query execution
</commit_message>
<xml_diff>
--- a/task/Mini-Project-Progress.xlsx
+++ b/task/Mini-Project-Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Batches\RSSoftTech\AdvJava-091125\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC1DD69-23BB-4C3F-A887-DFD38B5A3B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AE593-D7C0-48B7-9E75-F4725D653576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Topic Name</t>
+  </si>
+  <si>
+    <t>Avinash Jadhav</t>
+  </si>
+  <si>
+    <t>Sanket Chor</t>
+  </si>
+  <si>
+    <t>Harshwardhan Pachoute</t>
+  </si>
+  <si>
+    <t>Om Dighe</t>
+  </si>
+  <si>
+    <t>Pranit Vichare</t>
+  </si>
+  <si>
+    <t>Priyanka Rasal</t>
+  </si>
+  <si>
+    <t>Tajas Sutar</t>
+  </si>
+  <si>
+    <t>Deepak Dixit</t>
+  </si>
+  <si>
+    <t>Quick Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Musical Instrument </t>
   </si>
 </sst>
 </file>
@@ -348,25 +378,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>